<commit_message>
Refactor search, import, and export workflows
- Replaced `findBySearchCriteria` with enhanced `advancedSearch` method in `ManifestationRepository` to simplify parameters and improve query structure.
- Updated `FileServiceExportTest` and templates to reflect revised column mapping and added new classification (`class1`, `class2`) fields.
- Enhanced Amazon import logic to handle and automatically set material types (`Digital`, `Retail`) and additional classifications during processing.
- Introduced flexible view mode switching (`simple`, `multi`, `advanced`) for search forms with JavaScript-driven mode toggling.
- Improved data mapping and import performance in `AmazonImportService`.
- Updated tests to account for new search functionalities and classification fields in imports and exports.
- Refined templates and user interface for better UX in manifestation search and listing pages.
</commit_message>
<xml_diff>
--- a/tests/resources/importtest2.xlsx
+++ b/tests/resources/importtest2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">メモ</t>
   </si>
@@ -73,6 +73,12 @@
     <t xml:space="preserve">分類４</t>
   </si>
   <si>
+    <t xml:space="preserve">部類１</t>
+  </si>
+  <si>
+    <t xml:space="preserve">部類２</t>
+  </si>
+  <si>
     <t xml:space="preserve">場所１</t>
   </si>
   <si>
@@ -149,6 +155,12 @@
   </si>
   <si>
     <t xml:space="preserve">ぶんぶんぶん４</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndcx/999.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ndcy/123.456</t>
   </si>
   <si>
     <t xml:space="preserve">日本国内</t>
@@ -178,7 +190,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Noto Sans CJK JP"/>
@@ -216,6 +228,11 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Noto Sans Mono CJK JP"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
@@ -224,6 +241,7 @@
       <sz val="10"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -268,7 +286,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -294,10 +312,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -432,10 +454,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S3" activeCellId="0" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -498,10 +520,10 @@
       <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="6" t="s">
         <v>18</v>
       </c>
       <c r="T1" s="2" t="s">
@@ -527,94 +549,106 @@
       </c>
       <c r="AA1" s="2" t="s">
         <v>26</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" s="8" t="s">
         <v>37</v>
       </c>
+      <c r="K2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="M2" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="X2" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z2" s="1" t="n">
         <v>2025.1</v>
       </c>
-      <c r="Y2" s="1" t="n">
+      <c r="AA2" s="1" t="n">
         <v>1700</v>
       </c>
-      <c r="Z2" s="9" t="n">
+      <c r="AB2" s="10" t="n">
         <v>46003.4244444444</v>
       </c>
-      <c r="AA2" s="9" t="n">
+      <c r="AC2" s="10" t="n">
         <v>46003.4244444444</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="C3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="8"/>
+      <c r="G3" s="9"/>
       <c r="H3" s="1"/>
       <c r="I3" s="2"/>
     </row>

</xml_diff>